<commit_message>
fix table to excel library disponible at https://github.com/linways/table-to-excel
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Product</t>
   </si>
@@ -25,40 +25,37 @@
     <t>Classic Burger</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>38.70</t>
+  </si>
+  <si>
+    <t>Cheddar Bacon</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Cheddar Bacon</t>
+    <t>Double Bacon</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>31.80</t>
-  </si>
-  <si>
-    <t>Double Bacon</t>
-  </si>
-  <si>
     <t>37.80</t>
   </si>
   <si>
     <t>Crispy Bacon Burger</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>17.90</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>87.50</t>
+    <t>76.50</t>
   </si>
 </sst>
 </file>
@@ -459,15 +456,15 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -478,32 +475,32 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created clean all function
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Product</t>
   </si>
@@ -34,28 +34,37 @@
     <t>Cheddar Bacon</t>
   </si>
   <si>
-    <t/>
+    <t>6</t>
+  </si>
+  <si>
+    <t>95.40</t>
   </si>
   <si>
     <t>Double Bacon</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>37.80</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>245.70</t>
   </si>
   <si>
     <t>Crispy Bacon Burger</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>89.50</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>76.50</t>
+    <t>27</t>
+  </si>
+  <si>
+    <t>469.30</t>
   </si>
 </sst>
 </file>
@@ -467,40 +476,40 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>